<commit_message>
luban 删除 --export_test_data选项，新增 --export_exclude_tags选项
</commit_message>
<xml_diff>
--- a/DesignerConfigs/Datas/tag_datas/tag.xlsx
+++ b/DesignerConfigs/Datas/tag_datas/tag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\designerconfigs\datas\tag_datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\DesignerConfigs\Datas\tag_datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892DE0D1-A9BE-471D-BDD2-D58A729E7384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578D285C-116A-4EC9-80CF-D96A8630FD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30180" yWindow="4200" windowWidth="24120" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tb_role_csv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>##</t>
   </si>
@@ -36,20 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>faLse</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -78,11 +64,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>false</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>##</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>any</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>any</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -447,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -455,111 +445,89 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="C11" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="B13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="B14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>